<commit_message>
uhh...haven't committed in forever
</commit_message>
<xml_diff>
--- a/Data/fishing_fish2_province.xlsx
+++ b/Data/fishing_fish2_province.xlsx
@@ -49,12 +49,12 @@
     <sheet name="1981" sheetId="28" r:id="rId35"/>
     <sheet name="1980" sheetId="29" r:id="rId36"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4417" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4452" uniqueCount="432">
   <si>
     <t>1</t>
   </si>
@@ -1251,6 +1251,105 @@
   </si>
   <si>
     <t>Province</t>
+  </si>
+  <si>
+    <t xml:space="preserve">349 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">156 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,628 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,196 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,111 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">75,426 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">80,801 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,973 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,649 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,473 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,554 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,715 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">187,881 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">75,221 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,652 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,119 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">68,722 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,112 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">176,055 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">191,063 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">80,372 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,997 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,871 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,292 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,859 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,236 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,620 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,354 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">182,698 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,855 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,344 </t>
   </si>
 </sst>
 </file>
@@ -14551,7 +14650,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14790,8 +14889,8 @@
       <c r="C10" s="1">
         <v>41481</v>
       </c>
-      <c r="D10">
-        <v>111.542</v>
+      <c r="D10" s="1">
+        <v>111542</v>
       </c>
       <c r="E10" s="1">
         <v>23108</v>
@@ -21862,7 +21961,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21936,23 +22035,20 @@
       <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1">
-        <v>2988</v>
-      </c>
-      <c r="H2" s="2">
-        <v>57</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2">
-        <v>349</v>
-      </c>
-      <c r="K2" s="2">
-        <v>156</v>
-      </c>
-      <c r="L2" s="2">
-        <v>323</v>
+      <c r="H2">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>399</v>
+      </c>
+      <c r="K2" t="s">
+        <v>400</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -21974,23 +22070,23 @@
       <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="1">
-        <v>8318</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="1">
-        <v>13628</v>
-      </c>
-      <c r="K3" s="2">
-        <v>379</v>
-      </c>
-      <c r="L3" s="1">
-        <v>9196</v>
+      <c r="G3">
+        <v>81</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5355</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>401</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -22013,22 +22109,22 @@
         <v>2</v>
       </c>
       <c r="G4" s="1">
-        <v>99525</v>
+        <v>10198</v>
       </c>
       <c r="H4" s="1">
-        <v>10864</v>
-      </c>
-      <c r="I4" s="2">
-        <v>424</v>
-      </c>
-      <c r="J4" s="1">
-        <v>19111</v>
-      </c>
-      <c r="K4" s="1">
-        <v>75426</v>
-      </c>
-      <c r="L4" s="1">
-        <v>80801</v>
+        <v>12807</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>403</v>
+      </c>
+      <c r="K4" t="s">
+        <v>404</v>
+      </c>
+      <c r="L4" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -22048,22 +22144,19 @@
       <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="2">
-        <v>306</v>
-      </c>
-      <c r="H5" s="2">
-        <v>377</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="2">
-        <v>23</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="H5">
+        <v>432</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -22086,23 +22179,21 @@
       <c r="F6" s="2">
         <v>300</v>
       </c>
-      <c r="G6" s="3">
-        <v>32255</v>
-      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1">
-        <v>60450</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1">
-        <v>4973</v>
-      </c>
-      <c r="K6" s="1">
-        <v>35649</v>
-      </c>
-      <c r="L6" s="1">
-        <v>9473</v>
+        <v>79423</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>406</v>
+      </c>
+      <c r="K6" t="s">
+        <v>407</v>
+      </c>
+      <c r="L6" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -22125,22 +22216,22 @@
         <v>13231</v>
       </c>
       <c r="G7" s="1">
-        <v>87552</v>
+        <v>23368</v>
       </c>
       <c r="H7" s="1">
-        <v>125157</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2554</v>
-      </c>
-      <c r="J7" s="1">
-        <v>7715</v>
-      </c>
-      <c r="K7" s="1">
-        <v>187881</v>
-      </c>
-      <c r="L7" s="1">
-        <v>75221</v>
+        <v>504422</v>
+      </c>
+      <c r="I7" t="s">
+        <v>409</v>
+      </c>
+      <c r="J7" t="s">
+        <v>410</v>
+      </c>
+      <c r="K7" t="s">
+        <v>411</v>
+      </c>
+      <c r="L7" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -22163,22 +22254,22 @@
         <v>7498</v>
       </c>
       <c r="G8" s="1">
-        <v>6218</v>
+        <v>16989</v>
       </c>
       <c r="H8" s="1">
-        <v>16068</v>
-      </c>
-      <c r="I8" s="1">
-        <v>10652</v>
-      </c>
-      <c r="J8" s="1">
-        <v>15119</v>
-      </c>
-      <c r="K8" s="1">
-        <v>68722</v>
-      </c>
-      <c r="L8" s="1">
-        <v>37112</v>
+        <v>154211</v>
+      </c>
+      <c r="I8" t="s">
+        <v>413</v>
+      </c>
+      <c r="J8" t="s">
+        <v>414</v>
+      </c>
+      <c r="K8" t="s">
+        <v>415</v>
+      </c>
+      <c r="L8" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -22201,22 +22292,22 @@
         <v>2</v>
       </c>
       <c r="G9" s="1">
-        <v>84126</v>
+        <v>76574</v>
       </c>
       <c r="H9" s="1">
-        <v>3902</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="1">
-        <v>27004</v>
-      </c>
-      <c r="K9" s="1">
-        <v>176055</v>
-      </c>
-      <c r="L9" s="1">
-        <v>191063</v>
+        <v>121514</v>
+      </c>
+      <c r="I9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>417</v>
+      </c>
+      <c r="K9" t="s">
+        <v>418</v>
+      </c>
+      <c r="L9" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -22238,23 +22329,23 @@
       <c r="F10" s="1">
         <v>7499</v>
       </c>
-      <c r="G10" s="1">
-        <v>18662</v>
+      <c r="G10">
+        <v>338</v>
       </c>
       <c r="H10" s="1">
-        <v>3278</v>
-      </c>
-      <c r="I10" s="1">
-        <v>80372</v>
-      </c>
-      <c r="J10" s="1">
-        <v>19997</v>
-      </c>
-      <c r="K10" s="1">
-        <v>24871</v>
-      </c>
-      <c r="L10" s="1">
-        <v>25292</v>
+        <v>144725</v>
+      </c>
+      <c r="I10" t="s">
+        <v>420</v>
+      </c>
+      <c r="J10" t="s">
+        <v>421</v>
+      </c>
+      <c r="K10" t="s">
+        <v>422</v>
+      </c>
+      <c r="L10" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -22276,23 +22367,23 @@
       <c r="F11" s="2">
         <v>88</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2">
-        <v>144</v>
-      </c>
-      <c r="I11" s="1">
-        <v>34859</v>
-      </c>
-      <c r="J11" s="1">
-        <v>10236</v>
-      </c>
-      <c r="K11" s="1">
-        <v>13620</v>
-      </c>
-      <c r="L11" s="1">
-        <v>2354</v>
+      <c r="G11">
+        <v>163</v>
+      </c>
+      <c r="H11" s="1">
+        <v>31617</v>
+      </c>
+      <c r="I11" t="s">
+        <v>424</v>
+      </c>
+      <c r="J11" t="s">
+        <v>425</v>
+      </c>
+      <c r="K11" t="s">
+        <v>426</v>
+      </c>
+      <c r="L11" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -22314,23 +22405,23 @@
       <c r="F12" s="3">
         <v>12179</v>
       </c>
-      <c r="G12" s="1">
-        <v>14866</v>
+      <c r="G12">
+        <v>973</v>
       </c>
       <c r="H12" s="1">
-        <v>1398</v>
-      </c>
-      <c r="I12" s="1">
-        <v>182698</v>
-      </c>
-      <c r="J12" s="1">
-        <v>9001</v>
-      </c>
-      <c r="K12" s="1">
-        <v>9855</v>
-      </c>
-      <c r="L12" s="1">
-        <v>3344</v>
+        <v>138190</v>
+      </c>
+      <c r="I12" t="s">
+        <v>428</v>
+      </c>
+      <c r="J12" t="s">
+        <v>429</v>
+      </c>
+      <c r="K12" t="s">
+        <v>430</v>
+      </c>
+      <c r="L12" t="s">
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>